<commit_message>
Update Interface check in
</commit_message>
<xml_diff>
--- a/Documents/Customers/01. Sothyra Say/INV-001.xlsx
+++ b/Documents/Customers/01. Sothyra Say/INV-001.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16828"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Company\Quotation\CUS01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\RMS\Documents\Customers\01. Sothyra Say\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Price Quote'!$A$1:$M$67</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -346,14 +346,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="6">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
     <numFmt numFmtId="166" formatCode="%* #,##0.00_);"/>
     <numFmt numFmtId="167" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="169" formatCode="%* #,##0_);"/>
+    <numFmt numFmtId="168" formatCode="%* #,##0_);"/>
   </numFmts>
   <fonts count="22" x14ac:knownFonts="1">
     <font>
@@ -951,15 +951,6 @@
     <xf numFmtId="2" fontId="12" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -975,6 +966,99 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="12" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="12" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -985,9 +1069,6 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1002,90 +1083,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="12" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="12" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -1094,15 +1103,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1763,10 +1763,10 @@
       <c r="A5" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="81" t="s">
+      <c r="B5" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="82"/>
+      <c r="C5" s="79"/>
       <c r="D5" s="16"/>
       <c r="E5" s="17" t="s">
         <v>14</v>
@@ -1776,10 +1776,10 @@
       <c r="A6" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="81" t="s">
+      <c r="B6" s="78" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="82"/>
+      <c r="C6" s="79"/>
       <c r="D6" s="16"/>
       <c r="E6" s="17" t="s">
         <v>14</v>
@@ -1794,8 +1794,8 @@
       <c r="A8" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="83"/>
-      <c r="C8" s="83"/>
+      <c r="B8" s="80"/>
+      <c r="C8" s="80"/>
       <c r="D8" s="20"/>
       <c r="E8" s="21"/>
     </row>
@@ -1809,66 +1809,66 @@
       <c r="A10" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="81">
+      <c r="B10" s="78">
         <v>111</v>
       </c>
-      <c r="C10" s="82"/>
+      <c r="C10" s="79"/>
       <c r="D10" s="16"/>
     </row>
     <row r="11" spans="1:5" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="81" t="s">
+      <c r="B11" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="82"/>
+      <c r="C11" s="79"/>
       <c r="D11" s="16"/>
     </row>
     <row r="12" spans="1:5" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="81" t="s">
+      <c r="B12" s="78" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="82"/>
+      <c r="C12" s="79"/>
       <c r="D12" s="16"/>
     </row>
     <row r="13" spans="1:5" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="81" t="s">
+      <c r="B13" s="78" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="82"/>
-      <c r="D13" s="84" t="s">
+      <c r="C13" s="79"/>
+      <c r="D13" s="81" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="85"/>
+      <c r="E13" s="82"/>
     </row>
     <row r="14" spans="1:5" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="81" t="s">
+      <c r="B14" s="78" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="82"/>
-      <c r="D14" s="84" t="s">
+      <c r="C14" s="79"/>
+      <c r="D14" s="81" t="s">
         <v>23</v>
       </c>
-      <c r="E14" s="85"/>
+      <c r="E14" s="82"/>
     </row>
     <row r="15" spans="1:5" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="78" t="s">
+      <c r="B15" s="83" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="79"/>
+      <c r="C15" s="84"/>
       <c r="D15" s="22"/>
     </row>
     <row r="16" spans="1:5" s="18" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -1880,40 +1880,40 @@
       <c r="A17" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="78" t="s">
+      <c r="B17" s="83" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="79"/>
+      <c r="C17" s="84"/>
       <c r="D17" s="22"/>
     </row>
     <row r="18" spans="1:5" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="78" t="s">
+      <c r="B18" s="83" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="79"/>
+      <c r="C18" s="84"/>
       <c r="D18" s="22"/>
     </row>
     <row r="19" spans="1:5" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="80" t="s">
+      <c r="B19" s="85" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="79"/>
+      <c r="C19" s="84"/>
       <c r="D19" s="22"/>
     </row>
     <row r="20" spans="1:5" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="80" t="s">
+      <c r="B20" s="85" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="79"/>
+      <c r="C20" s="84"/>
       <c r="D20" s="22"/>
     </row>
     <row r="21" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.2">
@@ -1925,20 +1925,20 @@
       <c r="A22" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="81" t="s">
+      <c r="B22" s="78" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="82"/>
+      <c r="C22" s="79"/>
       <c r="D22" s="16"/>
     </row>
     <row r="23" spans="1:5" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="78" t="s">
+      <c r="B23" s="83" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="79"/>
+      <c r="C23" s="84"/>
       <c r="D23" s="22"/>
     </row>
     <row r="24" spans="1:5" s="18" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -2001,23 +2001,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="D13:E13"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B22:C22"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <dataValidations count="4">
@@ -2047,8 +2047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T67"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17:T21"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M55" sqref="M55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2136,75 +2136,75 @@
       <c r="D8" s="6"/>
     </row>
     <row r="9" spans="1:20" s="33" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="112" t="s">
+      <c r="A9" s="110" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="113"/>
-      <c r="C9" s="113"/>
-      <c r="D9" s="113"/>
+      <c r="B9" s="111"/>
+      <c r="C9" s="111"/>
+      <c r="D9" s="111"/>
       <c r="E9" s="48"/>
       <c r="F9" s="46" t="s">
         <v>9</v>
       </c>
       <c r="G9" s="46"/>
-      <c r="H9" s="107">
+      <c r="H9" s="104">
         <f ca="1">TODAY()</f>
-        <v>42460</v>
-      </c>
-      <c r="I9" s="108"/>
-      <c r="J9" s="108"/>
-      <c r="K9" s="109"/>
+        <v>42500</v>
+      </c>
+      <c r="I9" s="105"/>
+      <c r="J9" s="105"/>
+      <c r="K9" s="106"/>
       <c r="L9" s="74"/>
       <c r="M9" s="74"/>
     </row>
     <row r="10" spans="1:20" s="33" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="111" t="s">
+      <c r="A10" s="108" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="111"/>
-      <c r="C10" s="111"/>
-      <c r="D10" s="111"/>
+      <c r="B10" s="108"/>
+      <c r="C10" s="108"/>
+      <c r="D10" s="108"/>
       <c r="E10" s="48"/>
       <c r="F10" s="46" t="s">
         <v>101</v>
       </c>
-      <c r="H10" s="92" t="s">
+      <c r="H10" s="119" t="s">
         <v>102</v>
       </c>
-      <c r="I10" s="93"/>
-      <c r="J10" s="93"/>
-      <c r="K10" s="94"/>
+      <c r="I10" s="120"/>
+      <c r="J10" s="120"/>
+      <c r="K10" s="121"/>
       <c r="L10" s="76"/>
       <c r="M10" s="76"/>
     </row>
     <row r="11" spans="1:20" s="33" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="90" t="s">
+      <c r="A11" s="109" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="90"/>
-      <c r="C11" s="90"/>
-      <c r="D11" s="90"/>
+      <c r="B11" s="109"/>
+      <c r="C11" s="109"/>
+      <c r="D11" s="109"/>
       <c r="E11" s="48"/>
       <c r="F11" s="46" t="s">
         <v>7</v>
       </c>
       <c r="G11" s="46"/>
-      <c r="H11" s="107">
+      <c r="H11" s="104">
         <v>42490</v>
       </c>
-      <c r="I11" s="108"/>
-      <c r="J11" s="108"/>
-      <c r="K11" s="109"/>
+      <c r="I11" s="105"/>
+      <c r="J11" s="105"/>
+      <c r="K11" s="106"/>
       <c r="L11" s="76"/>
       <c r="M11" s="76"/>
     </row>
     <row r="12" spans="1:20" s="33" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="90" t="s">
+      <c r="A12" s="109" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="90"/>
-      <c r="C12" s="90"/>
-      <c r="D12" s="90"/>
+      <c r="B12" s="109"/>
+      <c r="C12" s="109"/>
+      <c r="D12" s="109"/>
       <c r="E12" s="48"/>
       <c r="F12" s="46" t="s">
         <v>103</v>
@@ -2220,12 +2220,12 @@
       <c r="M12" s="76"/>
     </row>
     <row r="13" spans="1:20" s="33" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="90" t="s">
+      <c r="A13" s="109" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="90"/>
-      <c r="C13" s="90"/>
-      <c r="D13" s="90"/>
+      <c r="B13" s="109"/>
+      <c r="C13" s="109"/>
+      <c r="D13" s="109"/>
       <c r="E13" s="48"/>
       <c r="F13" s="46" t="s">
         <v>44</v>
@@ -2241,21 +2241,21 @@
       <c r="M13" s="75"/>
     </row>
     <row r="14" spans="1:20" s="33" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="90" t="s">
+      <c r="A14" s="109" t="s">
         <v>95</v>
       </c>
-      <c r="B14" s="90"/>
-      <c r="C14" s="90"/>
-      <c r="D14" s="90"/>
+      <c r="B14" s="109"/>
+      <c r="C14" s="109"/>
+      <c r="D14" s="109"/>
       <c r="E14" s="48"/>
       <c r="F14" s="73"/>
       <c r="G14" s="73"/>
       <c r="H14" s="73"/>
       <c r="I14" s="73"/>
-      <c r="J14" s="110"/>
-      <c r="K14" s="110"/>
-      <c r="L14" s="110"/>
-      <c r="M14" s="110"/>
+      <c r="J14" s="107"/>
+      <c r="K14" s="107"/>
+      <c r="L14" s="107"/>
+      <c r="M14" s="107"/>
     </row>
     <row r="15" spans="1:20" ht="7.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="16" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2277,11 +2277,11 @@
       <c r="J16" s="57" t="s">
         <v>97</v>
       </c>
-      <c r="K16" s="106" t="s">
+      <c r="K16" s="125" t="s">
         <v>2</v>
       </c>
-      <c r="L16" s="106"/>
-      <c r="M16" s="106"/>
+      <c r="L16" s="125"/>
+      <c r="M16" s="125"/>
       <c r="P16" s="50"/>
       <c r="Q16" s="50"/>
       <c r="R16" s="50"/>
@@ -2307,16 +2307,16 @@
       <c r="J17" s="64">
         <v>600</v>
       </c>
-      <c r="K17" s="115">
+      <c r="K17" s="96">
         <v>600</v>
       </c>
-      <c r="L17" s="116"/>
-      <c r="M17" s="117"/>
-      <c r="P17" s="104"/>
-      <c r="Q17" s="104"/>
-      <c r="R17" s="104"/>
-      <c r="S17" s="104"/>
-      <c r="T17" s="104"/>
+      <c r="L17" s="97"/>
+      <c r="M17" s="98"/>
+      <c r="P17" s="112"/>
+      <c r="Q17" s="112"/>
+      <c r="R17" s="112"/>
+      <c r="S17" s="112"/>
+      <c r="T17" s="112"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" s="61" t="s">
@@ -2331,14 +2331,14 @@
       <c r="H18" s="47"/>
       <c r="I18" s="63"/>
       <c r="J18" s="63"/>
-      <c r="K18" s="98"/>
-      <c r="L18" s="99"/>
-      <c r="M18" s="100"/>
-      <c r="P18" s="105"/>
-      <c r="Q18" s="105"/>
-      <c r="R18" s="105"/>
-      <c r="S18" s="105"/>
-      <c r="T18" s="105"/>
+      <c r="K18" s="89"/>
+      <c r="L18" s="90"/>
+      <c r="M18" s="91"/>
+      <c r="P18" s="113"/>
+      <c r="Q18" s="113"/>
+      <c r="R18" s="113"/>
+      <c r="S18" s="113"/>
+      <c r="T18" s="113"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" s="61" t="s">
@@ -2353,14 +2353,14 @@
       <c r="H19" s="47"/>
       <c r="I19" s="63"/>
       <c r="J19" s="63"/>
-      <c r="K19" s="98"/>
-      <c r="L19" s="99"/>
-      <c r="M19" s="100"/>
-      <c r="P19" s="105"/>
-      <c r="Q19" s="105"/>
-      <c r="R19" s="105"/>
-      <c r="S19" s="105"/>
-      <c r="T19" s="105"/>
+      <c r="K19" s="89"/>
+      <c r="L19" s="90"/>
+      <c r="M19" s="91"/>
+      <c r="P19" s="113"/>
+      <c r="Q19" s="113"/>
+      <c r="R19" s="113"/>
+      <c r="S19" s="113"/>
+      <c r="T19" s="113"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" s="61" t="s">
@@ -2375,14 +2375,14 @@
       <c r="H20" s="47"/>
       <c r="I20" s="63"/>
       <c r="J20" s="63"/>
-      <c r="K20" s="98"/>
-      <c r="L20" s="99"/>
-      <c r="M20" s="100"/>
-      <c r="P20" s="105"/>
-      <c r="Q20" s="105"/>
-      <c r="R20" s="105"/>
-      <c r="S20" s="105"/>
-      <c r="T20" s="105"/>
+      <c r="K20" s="89"/>
+      <c r="L20" s="90"/>
+      <c r="M20" s="91"/>
+      <c r="P20" s="113"/>
+      <c r="Q20" s="113"/>
+      <c r="R20" s="113"/>
+      <c r="S20" s="113"/>
+      <c r="T20" s="113"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" s="61" t="s">
@@ -2397,14 +2397,14 @@
       <c r="H21" s="47"/>
       <c r="I21" s="63"/>
       <c r="J21" s="63"/>
-      <c r="K21" s="98"/>
-      <c r="L21" s="99"/>
-      <c r="M21" s="100"/>
-      <c r="P21" s="105"/>
-      <c r="Q21" s="105"/>
-      <c r="R21" s="105"/>
-      <c r="S21" s="105"/>
-      <c r="T21" s="105"/>
+      <c r="K21" s="89"/>
+      <c r="L21" s="90"/>
+      <c r="M21" s="91"/>
+      <c r="P21" s="113"/>
+      <c r="Q21" s="113"/>
+      <c r="R21" s="113"/>
+      <c r="S21" s="113"/>
+      <c r="T21" s="113"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" s="61" t="s">
@@ -2419,9 +2419,9 @@
       <c r="H22" s="47"/>
       <c r="I22" s="63"/>
       <c r="J22" s="63"/>
-      <c r="K22" s="98"/>
-      <c r="L22" s="99"/>
-      <c r="M22" s="100"/>
+      <c r="K22" s="89"/>
+      <c r="L22" s="90"/>
+      <c r="M22" s="91"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" s="61" t="s">
@@ -2436,9 +2436,9 @@
       <c r="H23" s="47"/>
       <c r="I23" s="63"/>
       <c r="J23" s="63"/>
-      <c r="K23" s="98"/>
-      <c r="L23" s="99"/>
-      <c r="M23" s="100"/>
+      <c r="K23" s="89"/>
+      <c r="L23" s="90"/>
+      <c r="M23" s="91"/>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" s="61" t="s">
@@ -2453,9 +2453,9 @@
       <c r="H24" s="47"/>
       <c r="I24" s="63"/>
       <c r="J24" s="63"/>
-      <c r="K24" s="98"/>
-      <c r="L24" s="99"/>
-      <c r="M24" s="100"/>
+      <c r="K24" s="89"/>
+      <c r="L24" s="90"/>
+      <c r="M24" s="91"/>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25" s="61" t="s">
@@ -2470,9 +2470,9 @@
       <c r="H25" s="47"/>
       <c r="I25" s="63"/>
       <c r="J25" s="63"/>
-      <c r="K25" s="98"/>
-      <c r="L25" s="99"/>
-      <c r="M25" s="100"/>
+      <c r="K25" s="89"/>
+      <c r="L25" s="90"/>
+      <c r="M25" s="91"/>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" s="61" t="s">
@@ -2487,9 +2487,9 @@
       <c r="H26" s="47"/>
       <c r="I26" s="63"/>
       <c r="J26" s="63"/>
-      <c r="K26" s="98"/>
-      <c r="L26" s="99"/>
-      <c r="M26" s="100"/>
+      <c r="K26" s="89"/>
+      <c r="L26" s="90"/>
+      <c r="M26" s="91"/>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A27" s="61" t="s">
@@ -2504,9 +2504,9 @@
       <c r="H27" s="47"/>
       <c r="I27" s="63"/>
       <c r="J27" s="63"/>
-      <c r="K27" s="98"/>
-      <c r="L27" s="99"/>
-      <c r="M27" s="100"/>
+      <c r="K27" s="89"/>
+      <c r="L27" s="90"/>
+      <c r="M27" s="91"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" s="61" t="s">
@@ -2521,9 +2521,9 @@
       <c r="H28" s="47"/>
       <c r="I28" s="63"/>
       <c r="J28" s="63"/>
-      <c r="K28" s="98"/>
-      <c r="L28" s="99"/>
-      <c r="M28" s="100"/>
+      <c r="K28" s="89"/>
+      <c r="L28" s="90"/>
+      <c r="M28" s="91"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A29" s="61" t="s">
@@ -2538,9 +2538,9 @@
       <c r="H29" s="47"/>
       <c r="I29" s="63"/>
       <c r="J29" s="63"/>
-      <c r="K29" s="98"/>
-      <c r="L29" s="99"/>
-      <c r="M29" s="100"/>
+      <c r="K29" s="89"/>
+      <c r="L29" s="90"/>
+      <c r="M29" s="91"/>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30" s="61" t="s">
@@ -2555,9 +2555,9 @@
       <c r="H30" s="47"/>
       <c r="I30" s="63"/>
       <c r="J30" s="63"/>
-      <c r="K30" s="98"/>
-      <c r="L30" s="99"/>
-      <c r="M30" s="100"/>
+      <c r="K30" s="89"/>
+      <c r="L30" s="90"/>
+      <c r="M30" s="91"/>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31" s="61" t="s">
@@ -2572,9 +2572,9 @@
       <c r="H31" s="47"/>
       <c r="I31" s="63"/>
       <c r="J31" s="63"/>
-      <c r="K31" s="98"/>
-      <c r="L31" s="99"/>
-      <c r="M31" s="100"/>
+      <c r="K31" s="89"/>
+      <c r="L31" s="90"/>
+      <c r="M31" s="91"/>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A32" s="61" t="s">
@@ -2589,9 +2589,9 @@
       <c r="H32" s="47"/>
       <c r="I32" s="63"/>
       <c r="J32" s="63"/>
-      <c r="K32" s="98"/>
-      <c r="L32" s="99"/>
-      <c r="M32" s="100"/>
+      <c r="K32" s="89"/>
+      <c r="L32" s="90"/>
+      <c r="M32" s="91"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="61" t="s">
@@ -2606,9 +2606,9 @@
       <c r="H33" s="47"/>
       <c r="I33" s="63"/>
       <c r="J33" s="63"/>
-      <c r="K33" s="98"/>
-      <c r="L33" s="99"/>
-      <c r="M33" s="100"/>
+      <c r="K33" s="89"/>
+      <c r="L33" s="90"/>
+      <c r="M33" s="91"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="61" t="s">
@@ -2623,9 +2623,9 @@
       <c r="H34" s="47"/>
       <c r="I34" s="63"/>
       <c r="J34" s="63"/>
-      <c r="K34" s="98"/>
-      <c r="L34" s="99"/>
-      <c r="M34" s="100"/>
+      <c r="K34" s="89"/>
+      <c r="L34" s="90"/>
+      <c r="M34" s="91"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="61" t="s">
@@ -2640,9 +2640,9 @@
       <c r="H35" s="47"/>
       <c r="I35" s="63"/>
       <c r="J35" s="63"/>
-      <c r="K35" s="98"/>
-      <c r="L35" s="99"/>
-      <c r="M35" s="100"/>
+      <c r="K35" s="89"/>
+      <c r="L35" s="90"/>
+      <c r="M35" s="91"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="61" t="s">
@@ -2657,9 +2657,9 @@
       <c r="H36" s="47"/>
       <c r="I36" s="63"/>
       <c r="J36" s="63"/>
-      <c r="K36" s="98"/>
-      <c r="L36" s="99"/>
-      <c r="M36" s="100"/>
+      <c r="K36" s="89"/>
+      <c r="L36" s="90"/>
+      <c r="M36" s="91"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="61" t="s">
@@ -2674,9 +2674,9 @@
       <c r="H37" s="47"/>
       <c r="I37" s="63"/>
       <c r="J37" s="63"/>
-      <c r="K37" s="98"/>
-      <c r="L37" s="99"/>
-      <c r="M37" s="100"/>
+      <c r="K37" s="89"/>
+      <c r="L37" s="90"/>
+      <c r="M37" s="91"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="61" t="s">
@@ -2691,9 +2691,9 @@
       <c r="H38" s="47"/>
       <c r="I38" s="63"/>
       <c r="J38" s="63"/>
-      <c r="K38" s="98"/>
-      <c r="L38" s="99"/>
-      <c r="M38" s="100"/>
+      <c r="K38" s="89"/>
+      <c r="L38" s="90"/>
+      <c r="M38" s="91"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="61" t="s">
@@ -2708,9 +2708,9 @@
       <c r="H39" s="47"/>
       <c r="I39" s="63"/>
       <c r="J39" s="63"/>
-      <c r="K39" s="98"/>
-      <c r="L39" s="99"/>
-      <c r="M39" s="100"/>
+      <c r="K39" s="89"/>
+      <c r="L39" s="90"/>
+      <c r="M39" s="91"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="61" t="s">
@@ -2725,9 +2725,9 @@
       <c r="H40" s="47"/>
       <c r="I40" s="63"/>
       <c r="J40" s="63"/>
-      <c r="K40" s="98"/>
-      <c r="L40" s="99"/>
-      <c r="M40" s="100"/>
+      <c r="K40" s="89"/>
+      <c r="L40" s="90"/>
+      <c r="M40" s="91"/>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" s="61" t="s">
@@ -2742,9 +2742,9 @@
       <c r="H41" s="47"/>
       <c r="I41" s="63"/>
       <c r="J41" s="63"/>
-      <c r="K41" s="98"/>
-      <c r="L41" s="99"/>
-      <c r="M41" s="100"/>
+      <c r="K41" s="89"/>
+      <c r="L41" s="90"/>
+      <c r="M41" s="91"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" s="61" t="s">
@@ -2759,9 +2759,9 @@
       <c r="H42" s="47"/>
       <c r="I42" s="63"/>
       <c r="J42" s="63"/>
-      <c r="K42" s="98"/>
-      <c r="L42" s="99"/>
-      <c r="M42" s="100"/>
+      <c r="K42" s="89"/>
+      <c r="L42" s="90"/>
+      <c r="M42" s="91"/>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" s="61" t="s">
@@ -2776,9 +2776,9 @@
       <c r="H43" s="47"/>
       <c r="I43" s="63"/>
       <c r="J43" s="63"/>
-      <c r="K43" s="98"/>
-      <c r="L43" s="99"/>
-      <c r="M43" s="100"/>
+      <c r="K43" s="89"/>
+      <c r="L43" s="90"/>
+      <c r="M43" s="91"/>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" s="61" t="s">
@@ -2793,9 +2793,9 @@
       <c r="H44" s="47"/>
       <c r="I44" s="63"/>
       <c r="J44" s="63"/>
-      <c r="K44" s="98"/>
-      <c r="L44" s="99"/>
-      <c r="M44" s="100"/>
+      <c r="K44" s="89"/>
+      <c r="L44" s="90"/>
+      <c r="M44" s="91"/>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" s="61" t="s">
@@ -2810,9 +2810,9 @@
       <c r="H45" s="47"/>
       <c r="I45" s="63"/>
       <c r="J45" s="63"/>
-      <c r="K45" s="118"/>
-      <c r="L45" s="119"/>
-      <c r="M45" s="120"/>
+      <c r="K45" s="99"/>
+      <c r="L45" s="100"/>
+      <c r="M45" s="101"/>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" s="61" t="s">
@@ -2827,9 +2827,9 @@
       <c r="H46" s="47"/>
       <c r="I46" s="63"/>
       <c r="J46" s="63"/>
-      <c r="K46" s="101"/>
-      <c r="L46" s="102"/>
-      <c r="M46" s="103"/>
+      <c r="K46" s="86"/>
+      <c r="L46" s="87"/>
+      <c r="M46" s="88"/>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" s="61" t="s">
@@ -2844,9 +2844,9 @@
       <c r="H47" s="47"/>
       <c r="I47" s="63"/>
       <c r="J47" s="63"/>
-      <c r="K47" s="101"/>
-      <c r="L47" s="102"/>
-      <c r="M47" s="103"/>
+      <c r="K47" s="86"/>
+      <c r="L47" s="87"/>
+      <c r="M47" s="88"/>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" s="65"/>
@@ -2859,9 +2859,9 @@
       <c r="H48" s="68"/>
       <c r="I48" s="67"/>
       <c r="J48" s="67"/>
-      <c r="K48" s="101"/>
-      <c r="L48" s="102"/>
-      <c r="M48" s="103"/>
+      <c r="K48" s="86"/>
+      <c r="L48" s="87"/>
+      <c r="M48" s="88"/>
     </row>
     <row r="49" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="36"/>
@@ -2876,22 +2876,22 @@
       <c r="J49" s="77" t="s">
         <v>105</v>
       </c>
-      <c r="K49" s="126">
+      <c r="K49" s="122">
         <v>0.2</v>
       </c>
-      <c r="L49" s="127"/>
-      <c r="M49" s="128"/>
+      <c r="L49" s="123"/>
+      <c r="M49" s="124"/>
     </row>
     <row r="50" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="123" t="s">
+      <c r="A50" s="126" t="s">
         <v>4</v>
       </c>
-      <c r="B50" s="124"/>
-      <c r="C50" s="124"/>
-      <c r="D50" s="124"/>
-      <c r="E50" s="124"/>
-      <c r="F50" s="124"/>
-      <c r="G50" s="125"/>
+      <c r="B50" s="127"/>
+      <c r="C50" s="127"/>
+      <c r="D50" s="127"/>
+      <c r="E50" s="127"/>
+      <c r="F50" s="127"/>
+      <c r="G50" s="128"/>
       <c r="H50" s="8"/>
       <c r="I50" s="8"/>
       <c r="J50" s="37" t="s">
@@ -2907,15 +2907,15 @@
       </c>
     </row>
     <row r="51" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="89" t="s">
+      <c r="A51" s="117" t="s">
         <v>60</v>
       </c>
-      <c r="B51" s="90"/>
-      <c r="C51" s="90"/>
-      <c r="D51" s="90"/>
-      <c r="E51" s="90"/>
-      <c r="F51" s="90"/>
-      <c r="G51" s="91"/>
+      <c r="B51" s="109"/>
+      <c r="C51" s="109"/>
+      <c r="D51" s="109"/>
+      <c r="E51" s="109"/>
+      <c r="F51" s="109"/>
+      <c r="G51" s="118"/>
       <c r="H51" s="43"/>
       <c r="I51" s="43"/>
       <c r="J51" s="37" t="s">
@@ -2931,37 +2931,37 @@
       </c>
     </row>
     <row r="52" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="89" t="s">
+      <c r="A52" s="117" t="s">
         <v>61</v>
       </c>
-      <c r="B52" s="90"/>
-      <c r="C52" s="90"/>
-      <c r="D52" s="90"/>
-      <c r="E52" s="90"/>
-      <c r="F52" s="90"/>
-      <c r="G52" s="91"/>
+      <c r="B52" s="109"/>
+      <c r="C52" s="109"/>
+      <c r="D52" s="109"/>
+      <c r="E52" s="109"/>
+      <c r="F52" s="109"/>
+      <c r="G52" s="118"/>
       <c r="H52" s="44"/>
       <c r="I52" s="44"/>
       <c r="J52" s="37" t="str">
         <f>Settings!$B$27&amp;" Rate"</f>
         <v>VAT Rate</v>
       </c>
-      <c r="K52" s="95">
+      <c r="K52" s="93">
         <v>0</v>
       </c>
-      <c r="L52" s="96"/>
-      <c r="M52" s="97"/>
+      <c r="L52" s="94"/>
+      <c r="M52" s="95"/>
     </row>
     <row r="53" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="89" t="s">
+      <c r="A53" s="117" t="s">
         <v>62</v>
       </c>
-      <c r="B53" s="90"/>
-      <c r="C53" s="90"/>
-      <c r="D53" s="90"/>
-      <c r="E53" s="90"/>
-      <c r="F53" s="90"/>
-      <c r="G53" s="91"/>
+      <c r="B53" s="109"/>
+      <c r="C53" s="109"/>
+      <c r="D53" s="109"/>
+      <c r="E53" s="109"/>
+      <c r="F53" s="109"/>
+      <c r="G53" s="118"/>
       <c r="H53" s="44"/>
       <c r="I53" s="44"/>
       <c r="J53" s="37" t="str">
@@ -2979,15 +2979,15 @@
       </c>
     </row>
     <row r="54" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="86" t="s">
+      <c r="A54" s="114" t="s">
         <v>63</v>
       </c>
-      <c r="B54" s="87"/>
-      <c r="C54" s="87"/>
-      <c r="D54" s="87"/>
-      <c r="E54" s="87"/>
-      <c r="F54" s="87"/>
-      <c r="G54" s="88"/>
+      <c r="B54" s="115"/>
+      <c r="C54" s="115"/>
+      <c r="D54" s="115"/>
+      <c r="E54" s="115"/>
+      <c r="F54" s="115"/>
+      <c r="G54" s="116"/>
       <c r="H54" s="44"/>
       <c r="I54" s="44"/>
       <c r="J54" s="45" t="s">
@@ -3099,15 +3099,15 @@
       </c>
       <c r="B61" s="35"/>
       <c r="C61" s="35"/>
-      <c r="E61" s="121"/>
-      <c r="F61" s="121"/>
-      <c r="G61" s="121"/>
-      <c r="J61" s="122" t="s">
+      <c r="E61" s="102"/>
+      <c r="F61" s="102"/>
+      <c r="G61" s="102"/>
+      <c r="J61" s="103" t="s">
         <v>57</v>
       </c>
-      <c r="K61" s="122"/>
-      <c r="L61" s="122"/>
-      <c r="M61" s="122"/>
+      <c r="K61" s="103"/>
+      <c r="L61" s="103"/>
+      <c r="M61" s="103"/>
     </row>
     <row r="62" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
@@ -3155,21 +3155,21 @@
       <c r="M64" s="49"/>
     </row>
     <row r="65" spans="1:13" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="114" t="s">
+      <c r="A65" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="B65" s="114"/>
-      <c r="C65" s="114"/>
-      <c r="D65" s="114"/>
-      <c r="E65" s="114"/>
-      <c r="F65" s="114"/>
-      <c r="G65" s="114"/>
-      <c r="H65" s="114"/>
-      <c r="I65" s="114"/>
-      <c r="J65" s="114"/>
-      <c r="K65" s="114"/>
-      <c r="L65" s="114"/>
-      <c r="M65" s="114"/>
+      <c r="B65" s="92"/>
+      <c r="C65" s="92"/>
+      <c r="D65" s="92"/>
+      <c r="E65" s="92"/>
+      <c r="F65" s="92"/>
+      <c r="G65" s="92"/>
+      <c r="H65" s="92"/>
+      <c r="I65" s="92"/>
+      <c r="J65" s="92"/>
+      <c r="K65" s="92"/>
+      <c r="L65" s="92"/>
+      <c r="M65" s="92"/>
     </row>
     <row r="66" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="53"/>
@@ -3203,13 +3203,37 @@
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="K47:M47"/>
-    <mergeCell ref="K44:M44"/>
-    <mergeCell ref="K39:M39"/>
-    <mergeCell ref="K40:M40"/>
-    <mergeCell ref="K41:M41"/>
-    <mergeCell ref="K42:M42"/>
-    <mergeCell ref="K43:M43"/>
+    <mergeCell ref="A54:G54"/>
+    <mergeCell ref="A52:G52"/>
+    <mergeCell ref="A51:G51"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="K49:M49"/>
+    <mergeCell ref="K32:M32"/>
+    <mergeCell ref="K33:M33"/>
+    <mergeCell ref="K34:M34"/>
+    <mergeCell ref="K48:M48"/>
+    <mergeCell ref="A53:G53"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="A50:G50"/>
+    <mergeCell ref="K35:M35"/>
+    <mergeCell ref="K36:M36"/>
+    <mergeCell ref="K37:M37"/>
+    <mergeCell ref="K38:M38"/>
+    <mergeCell ref="P17:T21"/>
+    <mergeCell ref="K22:M22"/>
+    <mergeCell ref="K24:M24"/>
+    <mergeCell ref="K25:M25"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="J14:M14"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A14:D14"/>
     <mergeCell ref="A65:M65"/>
     <mergeCell ref="K52:M52"/>
     <mergeCell ref="K17:M17"/>
@@ -3226,37 +3250,13 @@
     <mergeCell ref="E61:G61"/>
     <mergeCell ref="J61:M61"/>
     <mergeCell ref="K26:M26"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="J14:M14"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="P17:T21"/>
-    <mergeCell ref="K22:M22"/>
-    <mergeCell ref="K24:M24"/>
-    <mergeCell ref="K25:M25"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="K20:M20"/>
-    <mergeCell ref="A54:G54"/>
-    <mergeCell ref="A52:G52"/>
-    <mergeCell ref="A51:G51"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="K49:M49"/>
-    <mergeCell ref="K32:M32"/>
-    <mergeCell ref="K33:M33"/>
-    <mergeCell ref="K34:M34"/>
-    <mergeCell ref="K48:M48"/>
-    <mergeCell ref="A53:G53"/>
-    <mergeCell ref="K16:M16"/>
-    <mergeCell ref="A50:G50"/>
-    <mergeCell ref="K35:M35"/>
-    <mergeCell ref="K36:M36"/>
-    <mergeCell ref="K37:M37"/>
-    <mergeCell ref="K38:M38"/>
+    <mergeCell ref="K47:M47"/>
+    <mergeCell ref="K44:M44"/>
+    <mergeCell ref="K39:M39"/>
+    <mergeCell ref="K40:M40"/>
+    <mergeCell ref="K41:M41"/>
+    <mergeCell ref="K42:M42"/>
+    <mergeCell ref="K43:M43"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A50 A9:D9">

</xml_diff>